<commit_message>
revise K(part 2), L, Q-S replaceable brand list
</commit_message>
<xml_diff>
--- a/code/prep/raw/brand_in_name_Kp2_LQRS_final.xlsx
+++ b/code/prep/raw/brand_in_name_Kp2_LQRS_final.xlsx
@@ -12010,8 +12010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="E172" sqref="E172"/>
+    <sheetView tabSelected="1" topLeftCell="A464" workbookViewId="0">
+      <selection activeCell="E469" sqref="E469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8"/>
@@ -17259,7 +17259,7 @@
         <v>2084</v>
       </c>
       <c r="C471" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="472" spans="1:3">

</xml_diff>